<commit_message>
implemented all three methods
</commit_message>
<xml_diff>
--- a/td_ready.xlsx
+++ b/td_ready.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -42,22 +42,97 @@
     <x:t xml:space="preserve">Name</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Rank each of the following pitches, from highest to lowest</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">dtweddel@uwo.ca</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">David Tweddell</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Beta;Gamma;Delta;Alpha;Epsilon;</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Beta;Gamma;Delta;Epsilon;Alpha;</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Beta;Alpha;Gamma;Delta;Epsilon;</x:t>
+    <x:t xml:space="preserve">Rank each of the following pitches, starting with your most-preferred project at the top of the list.</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">ssmeltze@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sandra Christine Smeltzer</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">De Groot;Lee;Smye;Beveridge;McNair;Tang;Esses;Bitsuamlak;Hill;Petrella;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">abottere@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Andrew Botterell</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Lee;McNair;Smye;De Groot;Tang;Beveridge;Hill;Esses;Bitsuamlak;Petrella;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">litchfi@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">David William Litchfield</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tang;McNair;Smye;Lee;Petrella;De Groot;Beveridge;Hill;Esses;Bitsuamlak;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">joramcar@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Janis Cardy</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tang;Smye;Esses;De Groot;Lee;Hill;McNair;Petrella;Beveridge;Bitsuamlak;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">jburkell@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Jacquelyn Burkell</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Smye;Tang;Lee;Esses;McNair;De Groot;Hill;Bitsuamlak;Beveridge;Petrella;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">mcapretz@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Miriam Capretz</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Smye;Tang;De Groot;Petrella;Bitsuamlak;Esses;McNair;Beveridge;Hill;Lee;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">ascully2@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abbey Baran</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Petrella;Lee;McNair;De Groot;Smye;Beveridge;Bitsuamlak;Tang;Hill;Esses;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">bneff@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Bryan Neff</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Bitsuamlak;Lee;De Groot;Hill;McNair;Tang;Beveridge;Smye;Esses;Petrella;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">eabrams3@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Emily Ansari</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">McNair;Esses;De Groot;Lee;Bitsuamlak;Tang;Smye;Petrella;Hill;Beveridge;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">kenm@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Ken McRae</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Lee;Tang;Hill;De Groot;Esses;Smye;McNair;Beveridge;Petrella;Bitsuamlak;</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -154,15 +229,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F4" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:F4"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:F11"/>
   <x:tableColumns count="6">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
     <x:tableColumn id="3" uniqueName="3" name="Completion time" dataDxfId="3"/>
     <x:tableColumn id="4" uniqueName="4" name="Email" dataDxfId="0"/>
     <x:tableColumn id="5" uniqueName="5" name="Name" dataDxfId="0"/>
-    <x:tableColumn id="6" uniqueName="6" name="Rank each of the following pitches, from highest to lowest" dataDxfId="0"/>
+    <x:tableColumn id="6" uniqueName="6" name="Rank each of the following pitches, starting with your most-preferred project at the top of the list." dataDxfId="0"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -503,13 +578,13 @@
     </x:row>
     <x:row r="2" hidden="0">
       <x:c r="A2">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="2">
-        <x:v>44021.3676851852</x:v>
+        <x:v>44023.7712962963</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44021.3698032407</x:v>
+        <x:v>44023.773125</x:v>
       </x:c>
       <x:c r="D2" s="10" t="s">
         <x:v>6</x:v>
@@ -523,49 +598,189 @@
     </x:row>
     <x:row r="3" hidden="0">
       <x:c r="A3">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B3" s="2">
-        <x:v>44021.369837963</x:v>
+        <x:v>44024.4625925926</x:v>
       </x:c>
       <x:c r="C3" s="2">
-        <x:v>44021.3699189815</x:v>
+        <x:v>44024.4737384259</x:v>
       </x:c>
       <x:c r="D3" s="10" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="10" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F3" s="10" t="s">
-        <x:v>9</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" hidden="0">
       <x:c r="A4">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B4" s="2">
-        <x:v>44021.3699537037</x:v>
+        <x:v>44025.506087963</x:v>
       </x:c>
       <x:c r="C4" s="2">
-        <x:v>44021.3699884259</x:v>
+        <x:v>44025.5067708333</x:v>
       </x:c>
       <x:c r="D4" s="10" t="s">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E4" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F4" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" hidden="0">
+      <x:c r="A5">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="F4" s="10" t="s">
+      <x:c r="B5" s="2">
+        <x:v>44025.6872453704</x:v>
+      </x:c>
+      <x:c r="C5" s="2">
+        <x:v>44025.6879976852</x:v>
+      </x:c>
+      <x:c r="D5" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E5" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" hidden="0">
+      <x:c r="A6">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="2">
+        <x:v>44025.6959837963</x:v>
+      </x:c>
+      <x:c r="C6" s="2">
+        <x:v>44025.6978703704</x:v>
+      </x:c>
+      <x:c r="D6" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E6" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F6" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" hidden="0">
+      <x:c r="A7">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B7" s="2">
+        <x:v>44025.7209953704</x:v>
+      </x:c>
+      <x:c r="C7" s="2">
+        <x:v>44025.7305208333</x:v>
+      </x:c>
+      <x:c r="D7" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" hidden="0">
+      <x:c r="A8">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="B8" s="2">
+        <x:v>44026.3932060185</x:v>
+      </x:c>
+      <x:c r="C8" s="2">
+        <x:v>44026.4142476852</x:v>
+      </x:c>
+      <x:c r="D8" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E8" s="10" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="F8" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" hidden="0">
+      <x:c r="A9">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B9" s="2">
+        <x:v>44026.4249768518</x:v>
+      </x:c>
+      <x:c r="C9" s="2">
+        <x:v>44026.4394675926</x:v>
+      </x:c>
+      <x:c r="D9" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E9" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="F9" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" hidden="0">
+      <x:c r="A10">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B10" s="2">
+        <x:v>44026.4753009259</x:v>
+      </x:c>
+      <x:c r="C10" s="2">
+        <x:v>44026.5234259259</x:v>
+      </x:c>
+      <x:c r="D10" s="10" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E10" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F10" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" hidden="0">
+      <x:c r="A11">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B11" s="2">
+        <x:v>44026.6851967593</x:v>
+      </x:c>
+      <x:c r="C11" s="2">
+        <x:v>44026.8601736111</x:v>
+      </x:c>
+      <x:c r="D11" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E11" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F11" s="10" t="s">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R44f449ad0f9b45f3"/>
+    <x:tablePart r:id="R83f1d83ab8c84f23"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
split matrix voting readers into module
</commit_message>
<xml_diff>
--- a/td_ready.xlsx
+++ b/td_ready.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -133,6 +133,15 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Lee;Tang;Hill;De Groot;Esses;Smye;McNair;Beveridge;Petrella;Bitsuamlak;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">mzbarack@uwo.ca</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Mark Zbaracki</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Petrella;Smye;Tang;Esses;Lee;De Groot;Bitsuamlak;McNair;Beveridge;Hill;</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -229,8 +238,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F11" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:F11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F12" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:F12"/>
   <x:tableColumns count="6">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -776,11 +785,31 @@
         <x:v>35</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" hidden="0">
+      <x:c r="A12">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B12" s="2">
+        <x:v>44027.4429282407</x:v>
+      </x:c>
+      <x:c r="C12" s="2">
+        <x:v>44027.4474652778</x:v>
+      </x:c>
+      <x:c r="D12" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E12" s="10" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F12" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R83f1d83ab8c84f23"/>
+    <x:tablePart r:id="R8493c8db091b44b0"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>